<commit_message>
fixed error in carter_2005_temp_thresholds.xlsx
</commit_message>
<xml_diff>
--- a/data/temperature/carter_2005_temp_thresholds.xlsx
+++ b/data/temperature/carter_2005_temp_thresholds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikea\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\mra_redds_norwest\data\temperature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F92F4C7-29B6-445D-B2FB-05E5758CAF3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DB8A8B-A5BB-49BD-A99F-273C77D06D15}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="21">
   <si>
     <t>species</t>
   </si>
@@ -45,9 +45,6 @@
     <t>temp_c</t>
   </si>
   <si>
-    <t>Chinook</t>
-  </si>
-  <si>
     <t>adult_holding</t>
   </si>
   <si>
@@ -85,6 +82,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>chinook</t>
+  </si>
+  <si>
+    <t>steelhead</t>
   </si>
 </sst>
 </file>
@@ -92,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -125,7 +128,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,13 +411,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -443,10 +446,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>43936</v>
@@ -455,7 +458,7 @@
         <v>43983</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <v>3.3</v>
@@ -463,10 +466,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>43936</v>
@@ -475,7 +478,7 @@
         <v>43983</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>7.2</v>
@@ -483,10 +486,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>43936</v>
@@ -495,7 +498,7 @@
         <v>43983</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>14.5</v>
@@ -503,10 +506,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>43936</v>
@@ -515,7 +518,7 @@
         <v>43983</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>18</v>
@@ -523,10 +526,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>43936</v>
@@ -535,7 +538,7 @@
         <v>43983</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>20</v>
@@ -543,10 +546,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>44053</v>
@@ -555,7 +558,7 @@
         <v>44104</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <v>3.3</v>
@@ -563,10 +566,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>44053</v>
@@ -575,7 +578,7 @@
         <v>44104</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>7.2</v>
@@ -583,10 +586,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>44053</v>
@@ -595,7 +598,7 @@
         <v>44104</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>14.5</v>
@@ -603,10 +606,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1">
         <v>44053</v>
@@ -615,7 +618,7 @@
         <v>44104</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>18</v>
@@ -623,10 +626,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>44053</v>
@@ -635,7 +638,7 @@
         <v>44104</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11">
         <v>20</v>
@@ -643,10 +646,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>44075</v>
@@ -655,7 +658,7 @@
         <v>43922</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -663,10 +666,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1">
         <v>44075</v>
@@ -675,7 +678,7 @@
         <v>43922</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -683,10 +686,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <v>44075</v>
@@ -695,7 +698,7 @@
         <v>43922</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>11</v>
@@ -703,10 +706,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>44075</v>
@@ -715,7 +718,7 @@
         <v>43922</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -723,10 +726,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1">
         <v>44075</v>
@@ -735,7 +738,7 @@
         <v>43922</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16">
         <v>17.5</v>
@@ -743,10 +746,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>43891</v>
@@ -755,7 +758,7 @@
         <v>43922</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -763,10 +766,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1">
         <v>43891</v>
@@ -775,7 +778,7 @@
         <v>43922</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -783,10 +786,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1">
         <v>43891</v>
@@ -795,7 +798,7 @@
         <v>43922</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -803,10 +806,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1">
         <v>43891</v>
@@ -815,7 +818,7 @@
         <v>43922</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <v>16.7</v>
@@ -823,10 +826,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="1">
         <v>43891</v>
@@ -835,7 +838,7 @@
         <v>43922</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21">
         <v>17.5</v>
@@ -843,10 +846,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1">
         <v>43992</v>
@@ -855,7 +858,7 @@
         <v>44119</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22">
         <v>4.5</v>
@@ -863,10 +866,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1">
         <v>43992</v>
@@ -875,7 +878,7 @@
         <v>44119</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -883,10 +886,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1">
         <v>43992</v>
@@ -895,7 +898,7 @@
         <v>44119</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24">
         <v>16</v>
@@ -903,10 +906,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
         <v>43992</v>
@@ -915,7 +918,7 @@
         <v>44119</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25">
         <v>20</v>
@@ -923,10 +926,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="1">
         <v>43992</v>
@@ -935,7 +938,7 @@
         <v>44119</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26">
         <v>22</v>
@@ -943,10 +946,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1">
         <v>44149</v>
@@ -955,7 +958,7 @@
         <v>43891</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27">
         <v>4.5</v>
@@ -963,10 +966,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1">
         <v>44149</v>
@@ -975,7 +978,7 @@
         <v>43891</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28">
         <v>10</v>
@@ -983,10 +986,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1">
         <v>44149</v>
@@ -995,7 +998,7 @@
         <v>43891</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29">
         <v>16</v>
@@ -1003,10 +1006,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1">
         <v>44149</v>
@@ -1015,7 +1018,7 @@
         <v>43891</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30">
         <v>20</v>
@@ -1023,10 +1026,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1">
         <v>44149</v>
@@ -1035,7 +1038,7 @@
         <v>43891</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31">
         <v>22</v>
@@ -1043,10 +1046,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1">
         <v>43891</v>
@@ -1055,7 +1058,7 @@
         <v>43991</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32">
         <v>4.5</v>
@@ -1063,10 +1066,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1">
         <v>43891</v>
@@ -1075,7 +1078,7 @@
         <v>43991</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33">
         <v>10</v>
@@ -1083,10 +1086,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1">
         <v>43891</v>
@@ -1095,7 +1098,7 @@
         <v>43991</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34">
         <v>16</v>
@@ -1103,10 +1106,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1">
         <v>43891</v>
@@ -1115,7 +1118,7 @@
         <v>43991</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F35">
         <v>20</v>
@@ -1123,10 +1126,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36" s="1">
         <v>43891</v>
@@ -1135,7 +1138,7 @@
         <v>43991</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F36">
         <v>22</v>
@@ -1143,10 +1146,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
         <v>6</v>
-      </c>
-      <c r="B37" t="s">
-        <v>7</v>
       </c>
       <c r="C37" s="1">
         <v>44105</v>
@@ -1155,18 +1158,18 @@
         <v>43921</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
         <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
       </c>
       <c r="C38" s="1">
         <v>44105</v>
@@ -1175,18 +1178,18 @@
         <v>43921</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
         <v>6</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
       </c>
       <c r="C39" s="1">
         <v>44105</v>
@@ -1195,18 +1198,18 @@
         <v>43921</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
         <v>6</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
       </c>
       <c r="C40" s="1">
         <v>44105</v>
@@ -1215,7 +1218,7 @@
         <v>43921</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40">
         <v>18</v>
@@ -1223,10 +1226,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
         <v>6</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
       </c>
       <c r="C41" s="1">
         <v>44105</v>
@@ -1235,7 +1238,7 @@
         <v>43921</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -1243,10 +1246,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42" s="1">
         <v>43922</v>
@@ -1255,18 +1258,18 @@
         <v>43982</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" s="1">
         <v>43922</v>
@@ -1275,7 +1278,7 @@
         <v>43982</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43">
         <v>3.9</v>
@@ -1283,10 +1286,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1">
         <v>43922</v>
@@ -1295,7 +1298,7 @@
         <v>43982</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44">
         <v>12.8</v>
@@ -1303,10 +1306,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C45" s="1">
         <v>43922</v>
@@ -1315,7 +1318,7 @@
         <v>43982</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45">
         <v>18</v>
@@ -1323,10 +1326,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" s="1">
         <v>43922</v>
@@ -1335,7 +1338,7 @@
         <v>43982</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F46">
         <v>20</v>
@@ -1343,10 +1346,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1">
         <v>43922</v>
@@ -1355,7 +1358,7 @@
         <v>44013</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -1363,10 +1366,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C48" s="1">
         <v>43922</v>
@@ -1375,7 +1378,7 @@
         <v>44013</v>
       </c>
       <c r="E48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48">
         <v>5</v>
@@ -1383,10 +1386,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C49" s="1">
         <v>43922</v>
@@ -1395,7 +1398,7 @@
         <v>44013</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49">
         <v>10</v>
@@ -1403,10 +1406,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50" s="1">
         <v>43922</v>
@@ -1415,7 +1418,7 @@
         <v>44013</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50">
         <v>12</v>
@@ -1423,10 +1426,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C51" s="1">
         <v>43922</v>
@@ -1435,7 +1438,7 @@
         <v>44013</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F51">
         <v>14</v>
@@ -1443,10 +1446,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C52" s="1">
         <v>43997</v>
@@ -1455,7 +1458,7 @@
         <v>44027</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -1463,10 +1466,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C53" s="1">
         <v>43997</v>
@@ -1475,7 +1478,7 @@
         <v>44027</v>
       </c>
       <c r="E53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53">
         <v>5</v>
@@ -1483,10 +1486,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C54" s="1">
         <v>43997</v>
@@ -1495,7 +1498,7 @@
         <v>44027</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54">
         <v>10</v>
@@ -1503,10 +1506,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C55" s="1">
         <v>43997</v>
@@ -1515,7 +1518,7 @@
         <v>44027</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F55">
         <v>12</v>
@@ -1523,10 +1526,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C56" s="1">
         <v>43997</v>
@@ -1535,7 +1538,7 @@
         <v>44027</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F56">
         <v>14</v>
@@ -1543,10 +1546,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C57" s="1">
         <v>43992</v>
@@ -1555,7 +1558,7 @@
         <v>44119</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57">
         <v>4.5</v>
@@ -1563,10 +1566,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C58" s="1">
         <v>43992</v>
@@ -1575,7 +1578,7 @@
         <v>44119</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58">
         <v>10</v>
@@ -1583,10 +1586,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C59" s="1">
         <v>43992</v>
@@ -1595,7 +1598,7 @@
         <v>44119</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59">
         <v>18</v>
@@ -1603,10 +1606,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C60" s="1">
         <v>43992</v>
@@ -1615,7 +1618,7 @@
         <v>44119</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F60">
         <v>19</v>
@@ -1623,10 +1626,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C61" s="1">
         <v>43992</v>
@@ -1635,7 +1638,7 @@
         <v>44119</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F61">
         <v>22</v>
@@ -1643,10 +1646,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C62" s="1">
         <v>44149</v>
@@ -1655,7 +1658,7 @@
         <v>43891</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62">
         <v>4.5</v>
@@ -1663,10 +1666,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C63" s="1">
         <v>44149</v>
@@ -1675,7 +1678,7 @@
         <v>43891</v>
       </c>
       <c r="E63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63">
         <v>10</v>
@@ -1683,10 +1686,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C64" s="1">
         <v>44149</v>
@@ -1695,7 +1698,7 @@
         <v>43891</v>
       </c>
       <c r="E64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64">
         <v>18</v>
@@ -1703,10 +1706,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C65" s="1">
         <v>44149</v>
@@ -1715,7 +1718,7 @@
         <v>43891</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F65">
         <v>19</v>
@@ -1723,10 +1726,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C66" s="1">
         <v>44149</v>
@@ -1735,7 +1738,7 @@
         <v>43891</v>
       </c>
       <c r="E66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F66">
         <v>22</v>
@@ -1743,10 +1746,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C67" s="1">
         <v>43891</v>
@@ -1755,7 +1758,7 @@
         <v>43991</v>
       </c>
       <c r="E67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67">
         <v>4.5</v>
@@ -1763,10 +1766,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C68" s="1">
         <v>43891</v>
@@ -1775,7 +1778,7 @@
         <v>43991</v>
       </c>
       <c r="E68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68">
         <v>10</v>
@@ -1783,10 +1786,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C69" s="1">
         <v>43891</v>
@@ -1795,7 +1798,7 @@
         <v>43991</v>
       </c>
       <c r="E69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69">
         <v>18</v>
@@ -1803,10 +1806,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70" s="1">
         <v>43891</v>
@@ -1815,7 +1818,7 @@
         <v>43991</v>
       </c>
       <c r="E70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F70">
         <v>19</v>
@@ -1823,10 +1826,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C71" s="1">
         <v>43891</v>
@@ -1835,7 +1838,7 @@
         <v>43991</v>
       </c>
       <c r="E71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F71">
         <v>22</v>

</xml_diff>

<commit_message>
summarized mcnyset data by rkm, done for night
</commit_message>
<xml_diff>
--- a/data/temperature/carter_2005_temp_thresholds.xlsx
+++ b/data/temperature/carter_2005_temp_thresholds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\mra_redds_norwest\data\temperature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DB8A8B-A5BB-49BD-A99F-273C77D06D15}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D59F56-5BAD-4482-B1CF-DEFFFF1920CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,12 +33,6 @@
     <t>life_stage</t>
   </si>
   <si>
-    <t>timing_start</t>
-  </si>
-  <si>
-    <t>timing_end</t>
-  </si>
-  <si>
     <t>threshhold</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>steelhead</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
   </si>
 </sst>
 </file>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:A71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,24 +432,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>43936</v>
@@ -458,7 +458,7 @@
         <v>43983</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>3.3</v>
@@ -466,10 +466,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>43936</v>
@@ -478,7 +478,7 @@
         <v>43983</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>7.2</v>
@@ -486,10 +486,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>43936</v>
@@ -498,7 +498,7 @@
         <v>43983</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>14.5</v>
@@ -506,10 +506,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>43936</v>
@@ -518,7 +518,7 @@
         <v>43983</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>18</v>
@@ -526,10 +526,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>43936</v>
@@ -538,7 +538,7 @@
         <v>43983</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>20</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>44053</v>
@@ -558,7 +558,7 @@
         <v>44104</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <v>3.3</v>
@@ -566,10 +566,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>44053</v>
@@ -578,7 +578,7 @@
         <v>44104</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8">
         <v>7.2</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>44053</v>
@@ -598,7 +598,7 @@
         <v>44104</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F9">
         <v>14.5</v>
@@ -606,10 +606,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
         <v>44053</v>
@@ -618,7 +618,7 @@
         <v>44104</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>18</v>
@@ -626,10 +626,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
         <v>44053</v>
@@ -638,7 +638,7 @@
         <v>44104</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>20</v>
@@ -646,10 +646,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
         <v>44075</v>
@@ -658,7 +658,7 @@
         <v>43922</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -666,10 +666,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>44075</v>
@@ -678,7 +678,7 @@
         <v>43922</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -686,10 +686,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>44075</v>
@@ -698,7 +698,7 @@
         <v>43922</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <v>11</v>
@@ -706,10 +706,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
         <v>44075</v>
@@ -718,7 +718,7 @@
         <v>43922</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -726,10 +726,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1">
         <v>44075</v>
@@ -738,7 +738,7 @@
         <v>43922</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>17.5</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1">
         <v>43891</v>
@@ -758,7 +758,7 @@
         <v>43922</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -766,10 +766,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
         <v>43891</v>
@@ -778,7 +778,7 @@
         <v>43922</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -786,10 +786,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1">
         <v>43891</v>
@@ -798,7 +798,7 @@
         <v>43922</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1">
         <v>43891</v>
@@ -818,7 +818,7 @@
         <v>43922</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <v>16.7</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1">
         <v>43891</v>
@@ -838,7 +838,7 @@
         <v>43922</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F21">
         <v>17.5</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1">
         <v>43992</v>
@@ -858,7 +858,7 @@
         <v>44119</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F22">
         <v>4.5</v>
@@ -866,10 +866,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
         <v>43992</v>
@@ -878,7 +878,7 @@
         <v>44119</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -886,10 +886,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1">
         <v>43992</v>
@@ -898,7 +898,7 @@
         <v>44119</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F24">
         <v>16</v>
@@ -906,10 +906,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1">
         <v>43992</v>
@@ -918,7 +918,7 @@
         <v>44119</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <v>20</v>
@@ -926,10 +926,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1">
         <v>43992</v>
@@ -938,7 +938,7 @@
         <v>44119</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F26">
         <v>22</v>
@@ -946,10 +946,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1">
         <v>44149</v>
@@ -958,7 +958,7 @@
         <v>43891</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F27">
         <v>4.5</v>
@@ -966,10 +966,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1">
         <v>44149</v>
@@ -978,7 +978,7 @@
         <v>43891</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F28">
         <v>10</v>
@@ -986,10 +986,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C29" s="1">
         <v>44149</v>
@@ -998,7 +998,7 @@
         <v>43891</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F29">
         <v>16</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C30" s="1">
         <v>44149</v>
@@ -1018,7 +1018,7 @@
         <v>43891</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F30">
         <v>20</v>
@@ -1026,10 +1026,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C31" s="1">
         <v>44149</v>
@@ -1038,7 +1038,7 @@
         <v>43891</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F31">
         <v>22</v>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C32" s="1">
         <v>43891</v>
@@ -1058,7 +1058,7 @@
         <v>43991</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F32">
         <v>4.5</v>
@@ -1066,10 +1066,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C33" s="1">
         <v>43891</v>
@@ -1078,7 +1078,7 @@
         <v>43991</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F33">
         <v>10</v>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C34" s="1">
         <v>43891</v>
@@ -1098,7 +1098,7 @@
         <v>43991</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F34">
         <v>16</v>
@@ -1106,10 +1106,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C35" s="1">
         <v>43891</v>
@@ -1118,7 +1118,7 @@
         <v>43991</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F35">
         <v>20</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C36" s="1">
         <v>43891</v>
@@ -1138,7 +1138,7 @@
         <v>43991</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F36">
         <v>22</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C37" s="1">
         <v>44105</v>
@@ -1158,18 +1158,18 @@
         <v>43921</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1">
         <v>44105</v>
@@ -1178,18 +1178,18 @@
         <v>43921</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1">
         <v>44105</v>
@@ -1198,18 +1198,18 @@
         <v>43921</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C40" s="1">
         <v>44105</v>
@@ -1218,7 +1218,7 @@
         <v>43921</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F40">
         <v>18</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41" s="1">
         <v>44105</v>
@@ -1238,7 +1238,7 @@
         <v>43921</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -1246,10 +1246,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1">
         <v>43922</v>
@@ -1258,18 +1258,18 @@
         <v>43982</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1">
         <v>43922</v>
@@ -1278,7 +1278,7 @@
         <v>43982</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F43">
         <v>3.9</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1">
         <v>43922</v>
@@ -1298,7 +1298,7 @@
         <v>43982</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F44">
         <v>12.8</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1">
         <v>43922</v>
@@ -1318,7 +1318,7 @@
         <v>43982</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F45">
         <v>18</v>
@@ -1326,10 +1326,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C46" s="1">
         <v>43922</v>
@@ -1338,7 +1338,7 @@
         <v>43982</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F46">
         <v>20</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C47" s="1">
         <v>43922</v>
@@ -1358,7 +1358,7 @@
         <v>44013</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C48" s="1">
         <v>43922</v>
@@ -1378,7 +1378,7 @@
         <v>44013</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F48">
         <v>5</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C49" s="1">
         <v>43922</v>
@@ -1398,7 +1398,7 @@
         <v>44013</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F49">
         <v>10</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C50" s="1">
         <v>43922</v>
@@ -1418,7 +1418,7 @@
         <v>44013</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F50">
         <v>12</v>
@@ -1426,10 +1426,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C51" s="1">
         <v>43922</v>
@@ -1438,7 +1438,7 @@
         <v>44013</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F51">
         <v>14</v>
@@ -1446,10 +1446,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C52" s="1">
         <v>43997</v>
@@ -1458,7 +1458,7 @@
         <v>44027</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -1466,10 +1466,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C53" s="1">
         <v>43997</v>
@@ -1478,7 +1478,7 @@
         <v>44027</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F53">
         <v>5</v>
@@ -1486,10 +1486,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C54" s="1">
         <v>43997</v>
@@ -1498,7 +1498,7 @@
         <v>44027</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F54">
         <v>10</v>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C55" s="1">
         <v>43997</v>
@@ -1518,7 +1518,7 @@
         <v>44027</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F55">
         <v>12</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C56" s="1">
         <v>43997</v>
@@ -1538,7 +1538,7 @@
         <v>44027</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F56">
         <v>14</v>
@@ -1546,10 +1546,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C57" s="1">
         <v>43992</v>
@@ -1558,7 +1558,7 @@
         <v>44119</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F57">
         <v>4.5</v>
@@ -1566,10 +1566,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C58" s="1">
         <v>43992</v>
@@ -1578,7 +1578,7 @@
         <v>44119</v>
       </c>
       <c r="E58" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F58">
         <v>10</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C59" s="1">
         <v>43992</v>
@@ -1598,7 +1598,7 @@
         <v>44119</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F59">
         <v>18</v>
@@ -1606,10 +1606,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C60" s="1">
         <v>43992</v>
@@ -1618,7 +1618,7 @@
         <v>44119</v>
       </c>
       <c r="E60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F60">
         <v>19</v>
@@ -1626,10 +1626,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C61" s="1">
         <v>43992</v>
@@ -1638,7 +1638,7 @@
         <v>44119</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F61">
         <v>22</v>
@@ -1646,10 +1646,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C62" s="1">
         <v>44149</v>
@@ -1658,7 +1658,7 @@
         <v>43891</v>
       </c>
       <c r="E62" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F62">
         <v>4.5</v>
@@ -1666,10 +1666,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C63" s="1">
         <v>44149</v>
@@ -1678,7 +1678,7 @@
         <v>43891</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F63">
         <v>10</v>
@@ -1686,10 +1686,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C64" s="1">
         <v>44149</v>
@@ -1698,7 +1698,7 @@
         <v>43891</v>
       </c>
       <c r="E64" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F64">
         <v>18</v>
@@ -1706,10 +1706,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C65" s="1">
         <v>44149</v>
@@ -1718,7 +1718,7 @@
         <v>43891</v>
       </c>
       <c r="E65" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F65">
         <v>19</v>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C66" s="1">
         <v>44149</v>
@@ -1738,7 +1738,7 @@
         <v>43891</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F66">
         <v>22</v>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C67" s="1">
         <v>43891</v>
@@ -1758,7 +1758,7 @@
         <v>43991</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F67">
         <v>4.5</v>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C68" s="1">
         <v>43891</v>
@@ -1778,7 +1778,7 @@
         <v>43991</v>
       </c>
       <c r="E68" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F68">
         <v>10</v>
@@ -1786,10 +1786,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C69" s="1">
         <v>43891</v>
@@ -1798,7 +1798,7 @@
         <v>43991</v>
       </c>
       <c r="E69" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F69">
         <v>18</v>
@@ -1806,10 +1806,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C70" s="1">
         <v>43891</v>
@@ -1818,7 +1818,7 @@
         <v>43991</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F70">
         <v>19</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C71" s="1">
         <v>43891</v>
@@ -1838,7 +1838,7 @@
         <v>43991</v>
       </c>
       <c r="E71" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F71">
         <v>22</v>

</xml_diff>

<commit_message>
fixed one last error in carter_2005_temp_thresholds.xlsx
</commit_message>
<xml_diff>
--- a/data/temperature/carter_2005_temp_thresholds.xlsx
+++ b/data/temperature/carter_2005_temp_thresholds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\mra_redds_norwest\data\temperature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D59F56-5BAD-4482-B1CF-DEFFFF1920CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E073F33-F5F8-4DC4-9DFC-4C5CFC72F3BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
damnit, misspelled threshold in carter_2005_temp_thresholds.xlsx; fixed
</commit_message>
<xml_diff>
--- a/data/temperature/carter_2005_temp_thresholds.xlsx
+++ b/data/temperature/carter_2005_temp_thresholds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\mra_redds_norwest\data\temperature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E073F33-F5F8-4DC4-9DFC-4C5CFC72F3BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574B4195-215E-4A0D-868C-E9BC4EAB47AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>life_stage</t>
   </si>
   <si>
-    <t>threshhold</t>
-  </si>
-  <si>
     <t>temp_c</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>end_date</t>
+  </si>
+  <si>
+    <t>threshold</t>
   </si>
 </sst>
 </file>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,24 +432,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>43936</v>
@@ -458,7 +458,7 @@
         <v>43983</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <v>3.3</v>
@@ -466,10 +466,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1">
         <v>43936</v>
@@ -478,7 +478,7 @@
         <v>43983</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <v>7.2</v>
@@ -486,10 +486,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
         <v>43936</v>
@@ -498,7 +498,7 @@
         <v>43983</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>14.5</v>
@@ -506,10 +506,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>43936</v>
@@ -518,7 +518,7 @@
         <v>43983</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5">
         <v>18</v>
@@ -526,10 +526,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>43936</v>
@@ -538,7 +538,7 @@
         <v>43983</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>20</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>44053</v>
@@ -558,7 +558,7 @@
         <v>44104</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>3.3</v>
@@ -566,10 +566,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <v>44053</v>
@@ -578,7 +578,7 @@
         <v>44104</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>7.2</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
         <v>44053</v>
@@ -598,7 +598,7 @@
         <v>44104</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9">
         <v>14.5</v>
@@ -606,10 +606,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
         <v>44053</v>
@@ -618,7 +618,7 @@
         <v>44104</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10">
         <v>18</v>
@@ -626,10 +626,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>44053</v>
@@ -638,7 +638,7 @@
         <v>44104</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <v>20</v>
@@ -646,10 +646,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>44075</v>
@@ -658,7 +658,7 @@
         <v>43922</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -666,10 +666,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
         <v>44075</v>
@@ -678,7 +678,7 @@
         <v>43922</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -686,10 +686,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
         <v>44075</v>
@@ -698,7 +698,7 @@
         <v>43922</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14">
         <v>11</v>
@@ -706,10 +706,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1">
         <v>44075</v>
@@ -718,7 +718,7 @@
         <v>43922</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -726,10 +726,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1">
         <v>44075</v>
@@ -738,7 +738,7 @@
         <v>43922</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>17.5</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
         <v>43891</v>
@@ -758,7 +758,7 @@
         <v>43922</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -766,10 +766,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1">
         <v>43891</v>
@@ -778,7 +778,7 @@
         <v>43922</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -786,10 +786,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1">
         <v>43891</v>
@@ -798,7 +798,7 @@
         <v>43922</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1">
         <v>43891</v>
@@ -818,7 +818,7 @@
         <v>43922</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20">
         <v>16.7</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1">
         <v>43891</v>
@@ -838,7 +838,7 @@
         <v>43922</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21">
         <v>17.5</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1">
         <v>43992</v>
@@ -858,7 +858,7 @@
         <v>44119</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <v>4.5</v>
@@ -866,10 +866,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
         <v>43992</v>
@@ -878,7 +878,7 @@
         <v>44119</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -886,10 +886,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
         <v>43992</v>
@@ -898,7 +898,7 @@
         <v>44119</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24">
         <v>16</v>
@@ -906,10 +906,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1">
         <v>43992</v>
@@ -918,7 +918,7 @@
         <v>44119</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25">
         <v>20</v>
@@ -926,10 +926,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1">
         <v>43992</v>
@@ -938,7 +938,7 @@
         <v>44119</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26">
         <v>22</v>
@@ -946,10 +946,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="1">
         <v>44149</v>
@@ -958,7 +958,7 @@
         <v>43891</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27">
         <v>4.5</v>
@@ -966,10 +966,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1">
         <v>44149</v>
@@ -978,7 +978,7 @@
         <v>43891</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28">
         <v>10</v>
@@ -986,10 +986,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1">
         <v>44149</v>
@@ -998,7 +998,7 @@
         <v>43891</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29">
         <v>16</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1">
         <v>44149</v>
@@ -1018,7 +1018,7 @@
         <v>43891</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30">
         <v>20</v>
@@ -1026,10 +1026,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="1">
         <v>44149</v>
@@ -1038,7 +1038,7 @@
         <v>43891</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31">
         <v>22</v>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="1">
         <v>43891</v>
@@ -1058,7 +1058,7 @@
         <v>43991</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32">
         <v>4.5</v>
@@ -1066,10 +1066,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="1">
         <v>43891</v>
@@ -1078,7 +1078,7 @@
         <v>43991</v>
       </c>
       <c r="E33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33">
         <v>10</v>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1">
         <v>43891</v>
@@ -1098,7 +1098,7 @@
         <v>43991</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34">
         <v>16</v>
@@ -1106,10 +1106,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" s="1">
         <v>43891</v>
@@ -1118,7 +1118,7 @@
         <v>43991</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35">
         <v>20</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="1">
         <v>43891</v>
@@ -1138,7 +1138,7 @@
         <v>43991</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36">
         <v>22</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" s="1">
         <v>44105</v>
@@ -1158,18 +1158,18 @@
         <v>43921</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1">
         <v>44105</v>
@@ -1178,18 +1178,18 @@
         <v>43921</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="1">
         <v>44105</v>
@@ -1198,18 +1198,18 @@
         <v>43921</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40" s="1">
         <v>44105</v>
@@ -1218,7 +1218,7 @@
         <v>43921</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40">
         <v>18</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="1">
         <v>44105</v>
@@ -1238,7 +1238,7 @@
         <v>43921</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -1246,10 +1246,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" s="1">
         <v>43922</v>
@@ -1258,18 +1258,18 @@
         <v>43982</v>
       </c>
       <c r="E42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C43" s="1">
         <v>43922</v>
@@ -1278,7 +1278,7 @@
         <v>43982</v>
       </c>
       <c r="E43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43">
         <v>3.9</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C44" s="1">
         <v>43922</v>
@@ -1298,7 +1298,7 @@
         <v>43982</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44">
         <v>12.8</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" s="1">
         <v>43922</v>
@@ -1318,7 +1318,7 @@
         <v>43982</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45">
         <v>18</v>
@@ -1326,10 +1326,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46" s="1">
         <v>43922</v>
@@ -1338,7 +1338,7 @@
         <v>43982</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46">
         <v>20</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C47" s="1">
         <v>43922</v>
@@ -1358,7 +1358,7 @@
         <v>44013</v>
       </c>
       <c r="E47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C48" s="1">
         <v>43922</v>
@@ -1378,7 +1378,7 @@
         <v>44013</v>
       </c>
       <c r="E48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48">
         <v>5</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C49" s="1">
         <v>43922</v>
@@ -1398,7 +1398,7 @@
         <v>44013</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49">
         <v>10</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C50" s="1">
         <v>43922</v>
@@ -1418,7 +1418,7 @@
         <v>44013</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50">
         <v>12</v>
@@ -1426,10 +1426,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" s="1">
         <v>43922</v>
@@ -1438,7 +1438,7 @@
         <v>44013</v>
       </c>
       <c r="E51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51">
         <v>14</v>
@@ -1446,10 +1446,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52" s="1">
         <v>43997</v>
@@ -1458,7 +1458,7 @@
         <v>44027</v>
       </c>
       <c r="E52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -1466,10 +1466,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" s="1">
         <v>43997</v>
@@ -1478,7 +1478,7 @@
         <v>44027</v>
       </c>
       <c r="E53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53">
         <v>5</v>
@@ -1486,10 +1486,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54" s="1">
         <v>43997</v>
@@ -1498,7 +1498,7 @@
         <v>44027</v>
       </c>
       <c r="E54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54">
         <v>10</v>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C55" s="1">
         <v>43997</v>
@@ -1518,7 +1518,7 @@
         <v>44027</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55">
         <v>12</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C56" s="1">
         <v>43997</v>
@@ -1538,7 +1538,7 @@
         <v>44027</v>
       </c>
       <c r="E56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56">
         <v>14</v>
@@ -1546,10 +1546,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C57" s="1">
         <v>43992</v>
@@ -1558,7 +1558,7 @@
         <v>44119</v>
       </c>
       <c r="E57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57">
         <v>4.5</v>
@@ -1566,10 +1566,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" s="1">
         <v>43992</v>
@@ -1578,7 +1578,7 @@
         <v>44119</v>
       </c>
       <c r="E58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58">
         <v>10</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" s="1">
         <v>43992</v>
@@ -1598,7 +1598,7 @@
         <v>44119</v>
       </c>
       <c r="E59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59">
         <v>18</v>
@@ -1606,10 +1606,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60" s="1">
         <v>43992</v>
@@ -1618,7 +1618,7 @@
         <v>44119</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60">
         <v>19</v>
@@ -1626,10 +1626,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" s="1">
         <v>43992</v>
@@ -1638,7 +1638,7 @@
         <v>44119</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F61">
         <v>22</v>
@@ -1646,10 +1646,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62" s="1">
         <v>44149</v>
@@ -1658,7 +1658,7 @@
         <v>43891</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62">
         <v>4.5</v>
@@ -1666,10 +1666,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C63" s="1">
         <v>44149</v>
@@ -1678,7 +1678,7 @@
         <v>43891</v>
       </c>
       <c r="E63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63">
         <v>10</v>
@@ -1686,10 +1686,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C64" s="1">
         <v>44149</v>
@@ -1698,7 +1698,7 @@
         <v>43891</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64">
         <v>18</v>
@@ -1706,10 +1706,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C65" s="1">
         <v>44149</v>
@@ -1718,7 +1718,7 @@
         <v>43891</v>
       </c>
       <c r="E65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65">
         <v>19</v>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C66" s="1">
         <v>44149</v>
@@ -1738,7 +1738,7 @@
         <v>43891</v>
       </c>
       <c r="E66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66">
         <v>22</v>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C67" s="1">
         <v>43891</v>
@@ -1758,7 +1758,7 @@
         <v>43991</v>
       </c>
       <c r="E67" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67">
         <v>4.5</v>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C68" s="1">
         <v>43891</v>
@@ -1778,7 +1778,7 @@
         <v>43991</v>
       </c>
       <c r="E68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68">
         <v>10</v>
@@ -1786,10 +1786,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C69" s="1">
         <v>43891</v>
@@ -1798,7 +1798,7 @@
         <v>43991</v>
       </c>
       <c r="E69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69">
         <v>18</v>
@@ -1806,10 +1806,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C70" s="1">
         <v>43891</v>
@@ -1818,7 +1818,7 @@
         <v>43991</v>
       </c>
       <c r="E70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70">
         <v>19</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C71" s="1">
         <v>43891</v>
@@ -1838,7 +1838,7 @@
         <v>43991</v>
       </c>
       <c r="E71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71">
         <v>22</v>

</xml_diff>